<commit_message>
Corrected script - TMTT0017341_EventExpense_VerifyTheCFExpenseRequestFunctionalityOfSearchFilters
</commit_message>
<xml_diff>
--- a/TestData/TMTT0017341_EventExpense_VerifyTheCFExpenseRequestFunctionalityOfSearchFilters.xlsx
+++ b/TestData/TMTT0017341_EventExpense_VerifyTheCFExpenseRequestFunctionalityOfSearchFilters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HL\SalesForce_Project\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D67AFF-2729-492D-8AAB-8F3ED60C8A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7E4F6A-AF8D-4B50-B4A4-2F604FD62481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
     <t>Leslie Ward</t>
   </si>
   <si>
-    <t>CF_Event123</t>
+    <t>PFG Golf Event</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>